<commit_message>
Weiterbau des Fahrzeuges, Code für das geradeaus Fahren geschreiben (Muss noch getestet werden)
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26DFF1F-F8F4-4ABA-82C4-1038962014E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA151A6B-CC1C-4D3B-830D-2A0B083C76AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="222">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1084,6 +1084,24 @@
   </si>
   <si>
     <t>Installation und Einrichtung von Sourcetree, Erstellen vom Github account und Verbindung mit dem Sourcetree, README Datei verändert und hochgeladen</t>
+  </si>
+  <si>
+    <t>Weiterbau des Fahrzeuges, Code für das Fahren des Fahrzeuges geschrieben (Muss getestet werden)</t>
+  </si>
+  <si>
+    <t>Umar</t>
+  </si>
+  <si>
+    <t>Berke</t>
+  </si>
+  <si>
+    <t>Berk</t>
+  </si>
+  <si>
+    <t>90% fertig</t>
+  </si>
+  <si>
+    <t>Ultraschallsensor Funktionsfähig, Infrarot muss noch eingebaut werden</t>
   </si>
 </sst>
 </file>
@@ -1785,6 +1803,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1803,32 +1845,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2339,14 +2357,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2395,10 +2413,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E7" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="112"/>
+      <c r="F7" s="107"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2407,8 +2425,8 @@
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2417,8 +2435,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2427,8 +2445,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2437,8 +2455,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2459,49 +2477,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="115"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="115"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="116"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2514,74 +2532,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111" t="s">
+      <c r="A23" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="112" t="s">
+      <c r="A26" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="112"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112" t="s">
+      <c r="B26" s="107"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="107" t="s">
+      <c r="A27" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="107"/>
-      <c r="C27" s="107"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="106" t="s">
+      <c r="A28" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="106"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="107" t="s">
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="108" t="s">
+      <c r="A29" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="108"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="109"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2592,6 +2600,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2651,7 +2669,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2665,11 +2683,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="121" t="s">
@@ -3486,8 +3504,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3501,16 +3519,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3677,13 +3695,23 @@
       <c r="B11" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
+      <c r="C11" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="57">
+        <v>5</v>
+      </c>
+      <c r="E11" s="56">
+        <v>5</v>
+      </c>
+      <c r="F11" s="56">
+        <v>2</v>
+      </c>
       <c r="G11" s="58"/>
       <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
+      <c r="I11" s="59" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
@@ -3692,10 +3720,18 @@
       <c r="B12" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="C12" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="57">
+        <v>3</v>
+      </c>
+      <c r="E12" s="56">
+        <v>1</v>
+      </c>
+      <c r="F12" s="56">
+        <v>2</v>
+      </c>
       <c r="G12" s="58"/>
       <c r="H12" s="58"/>
       <c r="I12" s="59"/>
@@ -3707,10 +3743,18 @@
       <c r="B13" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
+      <c r="C13" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="57">
+        <v>6</v>
+      </c>
+      <c r="E13" s="56">
+        <v>0</v>
+      </c>
+      <c r="F13" s="56">
+        <v>6</v>
+      </c>
       <c r="G13" s="58"/>
       <c r="H13" s="58"/>
       <c r="I13" s="59"/>
@@ -3722,10 +3766,18 @@
       <c r="B14" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
+      <c r="C14" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="57">
+        <v>3</v>
+      </c>
+      <c r="E14" s="56">
+        <v>1</v>
+      </c>
+      <c r="F14" s="56">
+        <v>2</v>
+      </c>
       <c r="G14" s="58"/>
       <c r="H14" s="56"/>
       <c r="I14" s="59"/>
@@ -3763,28 +3815,46 @@
       <c r="B17" s="55" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
+      <c r="C17" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="57">
+        <v>3</v>
+      </c>
+      <c r="E17" s="56">
+        <v>1</v>
+      </c>
+      <c r="F17" s="56">
+        <v>2</v>
+      </c>
       <c r="G17" s="58"/>
       <c r="H17" s="58"/>
       <c r="I17" s="59"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <v>32</v>
       </c>
       <c r="B18" s="55" t="s">
         <v>212</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
+      <c r="C18" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18" s="57">
+        <v>3</v>
+      </c>
+      <c r="E18" s="56">
+        <v>1</v>
+      </c>
+      <c r="F18" s="56">
+        <v>2</v>
+      </c>
       <c r="G18" s="58"/>
       <c r="H18" s="56"/>
-      <c r="I18" s="59"/>
+      <c r="I18" s="59" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
@@ -3849,10 +3919,18 @@
       <c r="B23" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
+      <c r="C23" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="D23" s="64">
+        <v>2</v>
+      </c>
+      <c r="E23" s="65">
+        <v>0</v>
+      </c>
+      <c r="F23" s="65">
+        <v>2</v>
+      </c>
       <c r="G23" s="58"/>
       <c r="H23" s="65"/>
       <c r="I23" s="66"/>
@@ -3864,10 +3942,18 @@
       <c r="B24" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
+      <c r="C24" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="64">
+        <v>1</v>
+      </c>
+      <c r="E24" s="65">
+        <v>0</v>
+      </c>
+      <c r="F24" s="65">
+        <v>1</v>
+      </c>
       <c r="G24" s="58"/>
       <c r="H24" s="65"/>
       <c r="I24" s="66"/>
@@ -3879,10 +3965,18 @@
       <c r="B25" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
+      <c r="C25" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="64">
+        <v>4</v>
+      </c>
+      <c r="E25" s="65">
+        <v>0</v>
+      </c>
+      <c r="F25" s="65">
+        <v>4</v>
+      </c>
       <c r="G25" s="58"/>
       <c r="H25" s="65"/>
       <c r="I25" s="66"/>
@@ -3894,10 +3988,18 @@
       <c r="B26" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
+      <c r="C26" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26" s="64">
+        <v>1</v>
+      </c>
+      <c r="E26" s="65">
+        <v>0</v>
+      </c>
+      <c r="F26" s="65">
+        <v>1</v>
+      </c>
       <c r="G26" s="58"/>
       <c r="H26" s="65"/>
       <c r="I26" s="66"/>
@@ -3909,10 +4011,18 @@
       <c r="B27" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
+      <c r="C27" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" s="64">
+        <v>4</v>
+      </c>
+      <c r="E27" s="65">
+        <v>0</v>
+      </c>
+      <c r="F27" s="65">
+        <v>1</v>
+      </c>
       <c r="G27" s="58"/>
       <c r="H27" s="65"/>
       <c r="I27" s="66"/>
@@ -3924,10 +4034,18 @@
       <c r="B28" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
+      <c r="C28" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="68">
+        <v>4</v>
+      </c>
+      <c r="E28" s="65">
+        <v>0</v>
+      </c>
+      <c r="F28" s="65">
+        <v>1</v>
+      </c>
       <c r="G28" s="58"/>
       <c r="H28" s="65"/>
       <c r="I28" s="66"/>
@@ -4009,15 +4127,15 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="49">
         <f>SUM(D10:D34)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I35" s="72"/>
     </row>
@@ -4030,8 +4148,8 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5626,7 +5744,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5688,10 +5806,16 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="2"/>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
+        <v>45257</v>
+      </c>
+      <c r="B7" s="41">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="41"/>

</xml_diff>

<commit_message>
Fertigstellungaufbau des Grundgerüsts des Fahrzeuges und halbwegs erfolgreiche Testung des Codes
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ESY_5AHEL_Car_09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA151A6B-CC1C-4D3B-830D-2A0B083C76AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F5940-2A45-4B79-92C0-65F64E017287}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="224">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1026,9 +1026,6 @@
     <t>Dauer [h]</t>
   </si>
   <si>
-    <t>Aufgabe / Thema</t>
-  </si>
-  <si>
     <t>Carkits auf Vollständigkeit geprüft</t>
   </si>
   <si>
@@ -1098,10 +1095,19 @@
     <t>Berk</t>
   </si>
   <si>
-    <t>90% fertig</t>
-  </si>
-  <si>
     <t>Ultraschallsensor Funktionsfähig, Infrarot muss noch eingebaut werden</t>
+  </si>
+  <si>
+    <t>Umar Abuev</t>
+  </si>
+  <si>
+    <t>Berke Bicici</t>
+  </si>
+  <si>
+    <t>Fahrzeug fertig aufgebaut (ohne Sensoren), Code für das Vorwärts fahren getestet (Halbwegs erfolgreich), Fehlersuche bei der Verkabelung (erfolgreich)</t>
+  </si>
+  <si>
+    <t>Montierung der letzten Bauteile. Fehlersuche der Verkabelungen. Organisierung der fehlenden Materialien für die Fertigstellung des Fahrzeuges</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1214,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1221,8 +1227,14 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1488,13 +1500,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1803,6 +1918,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1871,6 +1995,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2357,14 +2511,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="A1" s="109" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2413,10 +2567,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="107"/>
+      <c r="F7" s="110"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2425,8 +2579,8 @@
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2435,8 +2589,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2445,8 +2599,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2455,8 +2609,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2477,49 +2631,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="112"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="112"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="113"/>
-      <c r="C16" s="113"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="113"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="113"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="113"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="121"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2532,61 +2686,61 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="119" t="s">
+      <c r="A23" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="119"/>
-      <c r="C23" s="119"/>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="107"/>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107" t="s">
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="115" t="s">
+      <c r="A27" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="115"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="114" t="s">
+      <c r="A28" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="114"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="115" t="s">
-        <v>205</v>
-      </c>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118" t="s">
+        <v>204</v>
+      </c>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="117"/>
-      <c r="E29" s="117"/>
-      <c r="F29" s="117"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -2634,26 +2788,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="105" t="s">
         <v>198</v>
-      </c>
-      <c r="B1" s="105" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="104" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="104" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" s="104" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="104" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="104" t="s">
         <v>202</v>
-      </c>
-      <c r="B3" s="104" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2683,29 +2837,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="124" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="121"/>
+      <c r="C3" s="124"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="121"/>
+      <c r="C4" s="124"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="121"/>
+      <c r="C5" s="124"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2738,10 +2892,10 @@
         <v>20</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>206</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>207</v>
       </c>
       <c r="D10" s="30"/>
     </row>
@@ -2750,7 +2904,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>39</v>
@@ -2928,11 +3082,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -2940,18 +3094,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -2991,7 +3145,7 @@
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" s="39">
         <v>45257</v>
@@ -3219,14 +3373,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3504,8 +3658,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3519,16 +3673,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3615,7 +3769,7 @@
         <v>45236</v>
       </c>
       <c r="I6" s="59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
@@ -3696,22 +3850,20 @@
         <v>102</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D11" s="57">
         <v>5</v>
       </c>
       <c r="E11" s="56">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F11" s="56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="58"/>
       <c r="H11" s="58"/>
-      <c r="I11" s="59" t="s">
-        <v>220</v>
-      </c>
+      <c r="I11" s="59"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
@@ -3721,16 +3873,16 @@
         <v>103</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D12" s="57">
         <v>3</v>
       </c>
       <c r="E12" s="56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" s="56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="58"/>
       <c r="H12" s="58"/>
@@ -3744,16 +3896,16 @@
         <v>104</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" s="57">
         <v>6</v>
       </c>
       <c r="E13" s="56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G13" s="58"/>
       <c r="H13" s="58"/>
@@ -3767,7 +3919,7 @@
         <v>105</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D14" s="57">
         <v>3</v>
@@ -3813,10 +3965,10 @@
         <v>31</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D17" s="57">
         <v>3</v>
@@ -3836,10 +3988,10 @@
         <v>32</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D18" s="57">
         <v>3</v>
@@ -3853,7 +4005,7 @@
       <c r="G18" s="58"/>
       <c r="H18" s="56"/>
       <c r="I18" s="59" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3920,7 +4072,7 @@
         <v>110</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D23" s="64">
         <v>2</v>
@@ -3943,7 +4095,7 @@
         <v>111</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D24" s="64">
         <v>1</v>
@@ -3966,7 +4118,7 @@
         <v>112</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D25" s="64">
         <v>4</v>
@@ -3989,7 +4141,7 @@
         <v>113</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D26" s="64">
         <v>1</v>
@@ -4012,7 +4164,7 @@
         <v>114</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D27" s="64">
         <v>4</v>
@@ -4035,7 +4187,7 @@
         <v>115</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D28" s="68">
         <v>4</v>
@@ -4131,11 +4283,11 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I35" s="72"/>
     </row>
@@ -4181,19 +4333,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="128" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
@@ -4857,16 +5009,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="125" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -5642,71 +5794,71 @@
       <c r="A21" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="127" t="s">
+      <c r="B21" s="130" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="130"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="131" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="128"/>
+      <c r="C22" s="131"/>
+      <c r="D22" s="131"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="102" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="131" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
+      <c r="C23" s="131"/>
+      <c r="D23" s="131"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="128" t="s">
+      <c r="B24" s="131" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="131"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="99"/>
-      <c r="B25" s="126"/>
-      <c r="C25" s="126"/>
-      <c r="D25" s="126"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="99"/>
-      <c r="B26" s="126"/>
-      <c r="C26" s="126"/>
-      <c r="D26" s="126"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="99"/>
-      <c r="B27" s="126"/>
-      <c r="C27" s="126"/>
-      <c r="D27" s="126"/>
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="99"/>
-      <c r="B28" s="126"/>
-      <c r="C28" s="126"/>
-      <c r="D28" s="126"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="129"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="99"/>
-      <c r="B29" s="126"/>
-      <c r="C29" s="126"/>
-      <c r="D29" s="126"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5743,8 +5895,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5752,17 +5904,20 @@
     <col min="1" max="1" width="11.42578125" style="35"/>
     <col min="2" max="2" width="8.140625" style="35" customWidth="1"/>
     <col min="3" max="3" width="61.5703125" style="23" customWidth="1"/>
-    <col min="4" max="1024" width="11.42578125" style="23"/>
+    <col min="4" max="4" width="11.42578125" style="23"/>
+    <col min="5" max="5" width="31.42578125" style="23" customWidth="1"/>
+    <col min="6" max="1024" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-    </row>
-    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="125" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>194</v>
       </c>
@@ -5770,186 +5925,289 @@
         <v>195</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="D3" s="136" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="137"/>
+    </row>
+    <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>45188</v>
       </c>
       <c r="B4" s="103">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="108" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" s="138"/>
+      <c r="E4" s="139"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>45243</v>
       </c>
       <c r="B5" s="41">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="106" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>45250</v>
       </c>
       <c r="B6" s="41">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="106" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="140"/>
+      <c r="E6" s="141"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>45257</v>
       </c>
       <c r="B7" s="41">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="106" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="140"/>
+      <c r="E7" s="141"/>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>45264</v>
+      </c>
+      <c r="B8" s="41">
+        <v>3</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="133"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="41"/>
       <c r="B9" s="41"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="106"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="133"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="41"/>
       <c r="B10" s="41"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="106"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="41"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="106"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="41"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="106"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="133"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="106"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="133"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="41"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="106"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="41"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="106"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="41"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="106"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="41"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="106"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="41"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="106"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="133"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="41"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="106"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="133"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="106"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="106"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="133"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="106"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="133"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="106"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="106"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="133"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="106"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="133"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="106"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="133"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="106"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="133"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="41"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="106"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="133"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="106"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
       <c r="B30" s="41"/>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="106"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="133"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
       <c r="B31" s="41"/>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="106"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="133"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="41"/>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="106"/>
+      <c r="D32" s="132"/>
+      <c r="E32" s="133"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
-      <c r="C33" s="24"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="32">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fehlerbehebung der Motoren, Vervollständigung des Codes um Vorwärts zu fahren, Infrarotsensoren recherche betrieben
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ESY_5AHEL_Car_09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F5940-2A45-4B79-92C0-65F64E017287}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D694105-39A2-42E0-81B0-B307792F8949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="228">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1080,9 +1080,6 @@
     <t>Ultraschallsensor code für die Distanzmessung fertiggestellt und das Auto halbwegs fertig aufgebaut</t>
   </si>
   <si>
-    <t>Installation und Einrichtung von Sourcetree, Erstellen vom Github account und Verbindung mit dem Sourcetree, README Datei verändert und hochgeladen</t>
-  </si>
-  <si>
     <t>Weiterbau des Fahrzeuges, Code für das Fahren des Fahrzeuges geschrieben (Muss getestet werden)</t>
   </si>
   <si>
@@ -1108,6 +1105,21 @@
   </si>
   <si>
     <t>Montierung der letzten Bauteile. Fehlersuche der Verkabelungen. Organisierung der fehlenden Materialien für die Fertigstellung des Fahrzeuges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                               </t>
+  </si>
+  <si>
+    <t>Fehlerbehebung der Motoren, Code für das Vorwärts fahren vervollstänigt</t>
+  </si>
+  <si>
+    <t>Motoren richtig verlötet, Infrarotsensoren recherche betrieben</t>
+  </si>
+  <si>
+    <t>100% fertig</t>
+  </si>
+  <si>
+    <t>100% fertig ohne taster + sensoren</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1507,36 +1519,6 @@
       <right/>
       <top style="medium">
         <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1996,34 +1978,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3658,8 +3640,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L12:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3850,22 +3832,24 @@
         <v>102</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D11" s="57">
         <v>5</v>
       </c>
       <c r="E11" s="56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="56">
         <v>0</v>
       </c>
       <c r="G11" s="58"/>
       <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>22</v>
       </c>
@@ -3873,7 +3857,7 @@
         <v>103</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D12" s="57">
         <v>3</v>
@@ -3886,7 +3870,9 @@
       </c>
       <c r="G12" s="58"/>
       <c r="H12" s="58"/>
-      <c r="I12" s="59"/>
+      <c r="I12" s="59" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
@@ -3896,18 +3882,20 @@
         <v>104</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D13" s="57">
         <v>6</v>
       </c>
       <c r="E13" s="56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="56">
-        <v>3</v>
-      </c>
-      <c r="G13" s="58"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="58" t="s">
+        <v>28</v>
+      </c>
       <c r="H13" s="58"/>
       <c r="I13" s="59"/>
     </row>
@@ -3919,7 +3907,7 @@
         <v>105</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D14" s="57">
         <v>3</v>
@@ -3968,7 +3956,7 @@
         <v>210</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D17" s="57">
         <v>3</v>
@@ -3991,7 +3979,7 @@
         <v>211</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D18" s="57">
         <v>3</v>
@@ -4005,7 +3993,7 @@
       <c r="G18" s="58"/>
       <c r="H18" s="56"/>
       <c r="I18" s="59" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4072,7 +4060,7 @@
         <v>110</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D23" s="64">
         <v>2</v>
@@ -4095,7 +4083,7 @@
         <v>111</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D24" s="64">
         <v>1</v>
@@ -4118,7 +4106,7 @@
         <v>112</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D25" s="64">
         <v>4</v>
@@ -4141,7 +4129,7 @@
         <v>113</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D26" s="64">
         <v>1</v>
@@ -4164,7 +4152,7 @@
         <v>114</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D27" s="64">
         <v>4</v>
@@ -4187,7 +4175,7 @@
         <v>115</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D28" s="68">
         <v>4</v>
@@ -4283,11 +4271,11 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I35" s="72"/>
     </row>
@@ -5896,7 +5884,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+      <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5925,10 +5913,10 @@
         <v>195</v>
       </c>
       <c r="C3" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="136" t="s">
         <v>220</v>
-      </c>
-      <c r="D3" s="136" t="s">
-        <v>221</v>
       </c>
       <c r="E3" s="137"/>
     </row>
@@ -5945,7 +5933,7 @@
       <c r="D4" s="138"/>
       <c r="E4" s="139"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>45243</v>
       </c>
@@ -5955,10 +5943,12 @@
       <c r="C5" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="140"/>
+      <c r="D5" s="140" t="s">
+        <v>213</v>
+      </c>
       <c r="E5" s="141"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>45250</v>
       </c>
@@ -5966,7 +5956,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D6" s="140"/>
       <c r="E6" s="141"/>
@@ -5979,7 +5969,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="106" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D7" s="140"/>
       <c r="E7" s="141"/>
@@ -5992,18 +5982,26 @@
         <v>3</v>
       </c>
       <c r="C8" s="106" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="132" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="132" t="s">
-        <v>223</v>
-      </c>
       <c r="E8" s="133"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="132"/>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B9" s="41">
+        <v>3</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>225</v>
+      </c>
       <c r="E9" s="133"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Taster Aufgebaut udn Code geschrieben, Ultraschallsensor im Betriebnahme mit gerade aus fahren Erfolgreich
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D694105-39A2-42E0-81B0-B307792F8949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6958F093-E71D-4B56-9D00-4657FE438A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="231">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1120,6 +1120,15 @@
   </si>
   <si>
     <t>100% fertig ohne taster + sensoren</t>
+  </si>
+  <si>
+    <t>Ultraschallsensor code mit dem Vorwärtsfahren Code zusammen codiert, Tasten Vollständig aufgebaut und Code Vervollständigung</t>
+  </si>
+  <si>
+    <t>Das Auto fährt geradeaus mit Ultraschall und Taster</t>
+  </si>
+  <si>
+    <t>100% Fertig</t>
   </si>
 </sst>
 </file>
@@ -1909,12 +1918,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1924,36 +1963,6 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1984,29 +1993,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2493,14 +2502,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="120" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2549,10 +2558,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="110" t="s">
+      <c r="E7" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="110"/>
+      <c r="F7" s="115"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2561,8 +2570,8 @@
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2571,8 +2580,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2581,8 +2590,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2591,8 +2600,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2613,49 +2622,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="115"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="115"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="116"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2668,64 +2677,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="122"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
-      <c r="E23" s="122"/>
-      <c r="F23" s="122"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="114"/>
+      <c r="F23" s="114"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="110" t="s">
+      <c r="A26" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="110"/>
-      <c r="C26" s="110"/>
-      <c r="D26" s="110" t="s">
+      <c r="B26" s="115"/>
+      <c r="C26" s="115"/>
+      <c r="D26" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="110"/>
-      <c r="F26" s="110"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="115"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="118" t="s">
+      <c r="A27" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="117"/>
-      <c r="C28" s="117"/>
-      <c r="D28" s="118" t="s">
+      <c r="B28" s="109"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="119" t="s">
+      <c r="A29" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="119"/>
-      <c r="C29" s="119"/>
-      <c r="D29" s="120"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="120"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2736,16 +2755,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2819,11 +2828,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="124" t="s">
@@ -3640,8 +3649,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L12:L13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3655,16 +3664,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3888,16 +3897,18 @@
         <v>6</v>
       </c>
       <c r="E13" s="56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" s="56">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G13" s="58" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="58"/>
-      <c r="I13" s="59"/>
+      <c r="I13" s="59" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="28">
@@ -3913,14 +3924,16 @@
         <v>3</v>
       </c>
       <c r="E14" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="58"/>
       <c r="H14" s="56"/>
-      <c r="I14" s="59"/>
+      <c r="I14" s="59" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
@@ -4271,11 +4284,11 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I35" s="72"/>
     </row>
@@ -5884,7 +5897,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E9"/>
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5943,10 +5956,10 @@
       <c r="C5" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="140" t="s">
+      <c r="D5" s="134" t="s">
         <v>213</v>
       </c>
-      <c r="E5" s="141"/>
+      <c r="E5" s="135"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
@@ -5958,8 +5971,8 @@
       <c r="C6" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="140"/>
-      <c r="E6" s="141"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="135"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
@@ -5971,8 +5984,8 @@
       <c r="C7" s="106" t="s">
         <v>214</v>
       </c>
-      <c r="D7" s="140"/>
-      <c r="E7" s="141"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="135"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
@@ -6004,10 +6017,16 @@
       </c>
       <c r="E9" s="133"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="106"/>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B10" s="41">
+        <v>3</v>
+      </c>
+      <c r="C10" s="106" t="s">
+        <v>228</v>
+      </c>
       <c r="D10" s="132"/>
       <c r="E10" s="133"/>
     </row>
@@ -6169,11 +6188,34 @@
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
       <c r="C33" s="107"/>
-      <c r="D33" s="134"/>
-      <c r="E33" s="135"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
@@ -6183,29 +6225,6 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fehlerbehebung des Codes für das Vorwärtsfahren des Autos mit einem Start- und Stoptaster
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6958F093-E71D-4B56-9D00-4657FE438A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A6F6A4-DB34-40FB-9D7D-190B6E76C27A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="232">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1129,6 +1129,9 @@
   </si>
   <si>
     <t>100% Fertig</t>
+  </si>
+  <si>
+    <t>Fehlerbehebung des Codes für das Vorwärtsfahren des Autos mit einem Stop- und Starttaster</t>
   </si>
 </sst>
 </file>
@@ -1918,6 +1921,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1936,33 +1963,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1993,29 +1996,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2502,14 +2505,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2558,10 +2561,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="115" t="s">
+      <c r="E7" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="115"/>
+      <c r="F7" s="110"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2570,8 +2573,8 @@
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2580,8 +2583,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2590,8 +2593,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2600,8 +2603,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2622,49 +2625,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="121"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2677,74 +2680,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="114" t="s">
+      <c r="A23" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="114"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="114"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="115"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115" t="s">
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="109" t="s">
+      <c r="A28" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="110" t="s">
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="111" t="s">
+      <c r="A29" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2755,6 +2748,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2828,11 +2831,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="124" t="s">
@@ -3649,8 +3652,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3664,16 +3667,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4079,10 +4082,10 @@
         <v>2</v>
       </c>
       <c r="E23" s="65">
+        <v>1</v>
+      </c>
+      <c r="F23" s="65">
         <v>0</v>
-      </c>
-      <c r="F23" s="65">
-        <v>2</v>
       </c>
       <c r="G23" s="58"/>
       <c r="H23" s="65"/>
@@ -4284,11 +4287,11 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I35" s="72"/>
     </row>
@@ -5896,8 +5899,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5956,10 +5959,10 @@
       <c r="C5" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="134" t="s">
+      <c r="D5" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="E5" s="135"/>
+      <c r="E5" s="141"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
@@ -5971,8 +5974,8 @@
       <c r="C6" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="134"/>
-      <c r="E6" s="135"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="141"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
@@ -5984,8 +5987,8 @@
       <c r="C7" s="106" t="s">
         <v>214</v>
       </c>
-      <c r="D7" s="134"/>
-      <c r="E7" s="135"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="141"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
@@ -6030,10 +6033,16 @@
       <c r="D10" s="132"/>
       <c r="E10" s="133"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="106"/>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B11" s="41">
+        <v>1</v>
+      </c>
+      <c r="C11" s="106" t="s">
+        <v>231</v>
+      </c>
       <c r="D11" s="132"/>
       <c r="E11" s="133"/>
     </row>
@@ -6188,34 +6197,11 @@
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
       <c r="C33" s="107"/>
-      <c r="D33" s="140"/>
-      <c r="E33" s="141"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
@@ -6225,6 +6211,29 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Infrarotseonsor Code geschrieben, Fehler bei der Distanzmessung
</commit_message>
<xml_diff>
--- a/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
+++ b/Projekt-Steuerung_Autonom-Fahrendes-Auto_Vorgabe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Documents\group-09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\170443\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0C3DE9-B170-420F-A58D-E6A0823CB770}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBF6E19-1EA9-4506-AE84-14419BB65A0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="236">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1141,6 +1141,9 @@
   </si>
   <si>
     <t>An Diplomarbeit gearbeitet</t>
+  </si>
+  <si>
+    <t>Infrarotsensor Code geschrieben, Fehler bei der Messung der IR</t>
   </si>
 </sst>
 </file>
@@ -1930,6 +1933,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1948,33 +1975,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2005,29 +2008,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2514,14 +2517,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2570,10 +2573,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="115" t="s">
+      <c r="E7" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="115"/>
+      <c r="F7" s="110"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2582,8 +2585,8 @@
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2592,8 +2595,8 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2602,8 +2605,8 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2612,8 +2615,8 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2634,49 +2637,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119"/>
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="121"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2689,74 +2692,64 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="114" t="s">
+      <c r="A23" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="114"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="114"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="115"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115" t="s">
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="109" t="s">
+      <c r="A28" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="110" t="s">
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="111" t="s">
+      <c r="A29" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2767,6 +2760,16 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2840,11 +2843,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="124" t="s">
@@ -3676,16 +3679,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5909,7 +5912,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5970,10 +5973,10 @@
       <c r="C5" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="134" t="s">
+      <c r="D5" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="E5" s="135"/>
+      <c r="E5" s="141"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
@@ -5985,8 +5988,8 @@
       <c r="C6" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="134"/>
-      <c r="E6" s="135"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="141"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
@@ -5998,8 +6001,8 @@
       <c r="C7" s="106" t="s">
         <v>214</v>
       </c>
-      <c r="D7" s="134"/>
-      <c r="E7" s="135"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="141"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
@@ -6077,9 +6080,15 @@
       <c r="E12" s="133"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="106"/>
+      <c r="A13" s="40">
+        <v>44948</v>
+      </c>
+      <c r="B13" s="41">
+        <v>3</v>
+      </c>
+      <c r="C13" s="106" t="s">
+        <v>235</v>
+      </c>
       <c r="D13" s="132"/>
       <c r="E13" s="133"/>
     </row>
@@ -6220,34 +6229,11 @@
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
       <c r="C33" s="107"/>
-      <c r="D33" s="140"/>
-      <c r="E33" s="141"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
@@ -6257,6 +6243,29 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>